<commit_message>
Added solutions for math,dp and 2D arrays
</commit_message>
<xml_diff>
--- a/amazon_alltime.xlsx
+++ b/amazon_alltime.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kishor\Competative-Coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6507E9B-3D28-4454-B68F-431C62163DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419C2BFD-0556-4814-8E4E-4F10DB7B95F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="amazon_alltime" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2367" uniqueCount="1571">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2384" uniqueCount="1572">
   <si>
     <t>ID</t>
   </si>
@@ -4733,12 +4733,15 @@
   </si>
   <si>
     <t xml:space="preserve"> https://leetcode.com/problems/find-the-index-of-the-large-integer</t>
+  </si>
+  <si>
+    <t>Premium</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5573,11 +5576,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G781"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F38" sqref="F38"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="J88" sqref="J88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6405,6 +6408,9 @@
       <c r="F38" t="s">
         <v>84</v>
       </c>
+      <c r="G38" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
@@ -6468,6 +6474,9 @@
       <c r="F41" t="s">
         <v>90</v>
       </c>
+      <c r="G41" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
@@ -6548,6 +6557,9 @@
       <c r="F45" t="s">
         <v>98</v>
       </c>
+      <c r="G45" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
@@ -6568,6 +6580,9 @@
       <c r="F46" t="s">
         <v>100</v>
       </c>
+      <c r="G46" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
@@ -6609,7 +6624,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>909</v>
       </c>
@@ -6629,7 +6644,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>165</v>
       </c>
@@ -6649,7 +6664,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>56</v>
       </c>
@@ -6669,7 +6684,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>380</v>
       </c>
@@ -6689,7 +6704,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>53</v>
       </c>
@@ -6708,8 +6723,11 @@
       <c r="F53" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>49</v>
       </c>
@@ -6728,8 +6746,11 @@
       <c r="F54" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>545</v>
       </c>
@@ -6748,8 +6769,11 @@
       <c r="F55" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>11</v>
       </c>
@@ -6768,8 +6792,11 @@
       <c r="F56" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>76</v>
       </c>
@@ -6789,7 +6816,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>54</v>
       </c>
@@ -6808,8 +6835,11 @@
       <c r="F58" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>1152</v>
       </c>
@@ -6828,8 +6858,11 @@
       <c r="F59" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>45</v>
       </c>
@@ -6849,7 +6882,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>206</v>
       </c>
@@ -6868,8 +6901,11 @@
       <c r="F61" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>1167</v>
       </c>
@@ -6889,7 +6925,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>277</v>
       </c>
@@ -6909,7 +6945,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>124</v>
       </c>
@@ -6929,7 +6965,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>322</v>
       </c>
@@ -6949,7 +6985,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>863</v>
       </c>
@@ -6969,7 +7005,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>694</v>
       </c>
@@ -6989,7 +7025,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>103</v>
       </c>
@@ -7009,7 +7045,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>733</v>
       </c>
@@ -7028,8 +7064,11 @@
       <c r="F69" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>25</v>
       </c>
@@ -7049,7 +7088,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>341</v>
       </c>
@@ -7069,7 +7108,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>98</v>
       </c>
@@ -7088,8 +7127,11 @@
       <c r="F72" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G72" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>490</v>
       </c>
@@ -7109,7 +7151,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>208</v>
       </c>
@@ -7129,7 +7171,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>535</v>
       </c>
@@ -7149,7 +7191,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>1268</v>
       </c>
@@ -7169,7 +7211,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>224</v>
       </c>
@@ -7189,7 +7231,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>99</v>
       </c>
@@ -7209,7 +7251,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>289</v>
       </c>
@@ -7229,7 +7271,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>438</v>
       </c>
@@ -7249,7 +7291,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>116</v>
       </c>
@@ -7269,7 +7311,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>22</v>
       </c>
@@ -7289,7 +7331,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>218</v>
       </c>
@@ -7309,7 +7351,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>772</v>
       </c>
@@ -7329,7 +7371,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>314</v>
       </c>
@@ -7349,7 +7391,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>387</v>
       </c>
@@ -7368,8 +7410,11 @@
       <c r="F86" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G86" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>105</v>
       </c>
@@ -7388,8 +7433,11 @@
       <c r="F87" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G87" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>215</v>
       </c>
@@ -7409,7 +7457,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>102</v>
       </c>
@@ -7428,8 +7476,11 @@
       <c r="F89" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G89" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>207</v>
       </c>
@@ -7449,7 +7500,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>91</v>
       </c>
@@ -7469,7 +7520,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>140</v>
       </c>
@@ -7489,7 +7540,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>64</v>
       </c>
@@ -7508,8 +7559,11 @@
       <c r="F93" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G93" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>84</v>
       </c>
@@ -7529,7 +7583,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>866</v>
       </c>
@@ -7549,7 +7603,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Added solutions for linked lists and trees
</commit_message>
<xml_diff>
--- a/amazon_alltime.xlsx
+++ b/amazon_alltime.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kishor\Competative-Coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{419C2BFD-0556-4814-8E4E-4F10DB7B95F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E254B0DC-3C57-47CB-854D-591BAA41E249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2384" uniqueCount="1572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2398" uniqueCount="1572">
   <si>
     <t>ID</t>
   </si>
@@ -5579,8 +5579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G781"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="J88" sqref="J88"/>
+    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
+      <selection activeCell="F125" sqref="F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7150,6 +7150,9 @@
       <c r="F73" t="s">
         <v>154</v>
       </c>
+      <c r="G73" t="s">
+        <v>1571</v>
+      </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
@@ -7290,6 +7293,9 @@
       <c r="F80" t="s">
         <v>168</v>
       </c>
+      <c r="G80" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
@@ -7310,6 +7316,9 @@
       <c r="F81" t="s">
         <v>170</v>
       </c>
+      <c r="G81" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
@@ -7622,8 +7631,11 @@
       <c r="F96" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G96" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>227</v>
       </c>
@@ -7643,7 +7655,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>117</v>
       </c>
@@ -7663,7 +7675,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>505</v>
       </c>
@@ -7683,7 +7695,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>449</v>
       </c>
@@ -7703,7 +7715,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>55</v>
       </c>
@@ -7723,7 +7735,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>695</v>
       </c>
@@ -7743,7 +7755,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>362</v>
       </c>
@@ -7763,7 +7775,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>235</v>
       </c>
@@ -7782,8 +7794,11 @@
       <c r="F104" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G104" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>93</v>
       </c>
@@ -7802,8 +7817,11 @@
       <c r="F105" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G105" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>1000</v>
       </c>
@@ -7823,7 +7841,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>74</v>
       </c>
@@ -7842,8 +7860,11 @@
       <c r="F107" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G107" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>8</v>
       </c>
@@ -7863,7 +7884,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>1102</v>
       </c>
@@ -7883,7 +7904,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>221</v>
       </c>
@@ -7903,7 +7924,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>543</v>
       </c>
@@ -7922,8 +7943,11 @@
       <c r="F111" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G111" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>101</v>
       </c>
@@ -7942,8 +7966,11 @@
       <c r="F112" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G112" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>711</v>
       </c>
@@ -7962,8 +7989,11 @@
       <c r="F113" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G113" t="s">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>173</v>
       </c>
@@ -7983,7 +8013,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>445</v>
       </c>
@@ -8002,8 +8032,11 @@
       <c r="F115" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G115" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>143</v>
       </c>
@@ -8022,8 +8055,11 @@
       <c r="F116" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G116" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>31</v>
       </c>
@@ -8043,7 +8079,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>134</v>
       </c>
@@ -8063,7 +8099,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>234</v>
       </c>
@@ -8082,8 +8118,11 @@
       <c r="F119" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G119" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>199</v>
       </c>
@@ -8102,8 +8141,11 @@
       <c r="F120" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G120" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>72</v>
       </c>
@@ -8123,7 +8165,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>149</v>
       </c>
@@ -8143,7 +8185,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>79</v>
       </c>
@@ -8163,7 +8205,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>347</v>
       </c>
@@ -8183,7 +8225,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>62</v>
       </c>
@@ -8203,7 +8245,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>631</v>
       </c>
@@ -8223,7 +8265,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>394</v>
       </c>
@@ -8243,7 +8285,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>353</v>
       </c>

</xml_diff>

<commit_message>
Added solutions for stack, dp, dfs & bfs, trees and strings
</commit_message>
<xml_diff>
--- a/amazon_alltime.xlsx
+++ b/amazon_alltime.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Kishor\Competative-Coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E254B0DC-3C57-47CB-854D-591BAA41E249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9B552C-8AA2-48E2-BD67-77BEA19AF663}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="amazon_alltime" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2398" uniqueCount="1572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2405" uniqueCount="1573">
   <si>
     <t>ID</t>
   </si>
@@ -4736,6 +4736,9 @@
   </si>
   <si>
     <t>Premium</t>
+  </si>
+  <si>
+    <t>Total Solved</t>
   </si>
 </sst>
 </file>
@@ -5219,9 +5222,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -5577,19 +5586,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G781"/>
+  <dimension ref="A1:J781"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="F125" sqref="F125"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G146" sqref="G146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.42578125" customWidth="1"/>
     <col min="6" max="6" width="68.140625" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5612,7 +5622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>937</v>
       </c>
@@ -5632,7 +5642,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>200</v>
       </c>
@@ -5655,7 +5665,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1192</v>
       </c>
@@ -5675,7 +5685,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -5698,7 +5708,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>146</v>
       </c>
@@ -5718,7 +5728,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>973</v>
       </c>
@@ -5740,8 +5750,11 @@
       <c r="G7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J7" s="3" t="s">
+        <v>1572</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>819</v>
       </c>
@@ -5760,8 +5773,12 @@
       <c r="F8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J8" s="2">
+        <f>COUNTIF(G1:G800,"Done")</f>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>138</v>
       </c>
@@ -5781,7 +5798,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>5</v>
       </c>
@@ -5804,7 +5821,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>994</v>
       </c>
@@ -5827,7 +5844,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>42</v>
       </c>
@@ -5850,7 +5867,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>23</v>
       </c>
@@ -5873,7 +5890,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>763</v>
       </c>
@@ -5896,7 +5913,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -5919,7 +5936,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>20</v>
       </c>
@@ -8244,6 +8261,9 @@
       <c r="F125" t="s">
         <v>258</v>
       </c>
+      <c r="G125" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126">
@@ -8284,6 +8304,9 @@
       <c r="F127" t="s">
         <v>262</v>
       </c>
+      <c r="G127" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128">
@@ -8305,7 +8328,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>384</v>
       </c>
@@ -8325,7 +8348,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>323</v>
       </c>
@@ -8345,7 +8368,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>133</v>
       </c>
@@ -8365,7 +8388,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>706</v>
       </c>
@@ -8385,7 +8408,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>336</v>
       </c>
@@ -8405,7 +8428,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>682</v>
       </c>
@@ -8424,8 +8447,11 @@
       <c r="F134" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G134" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>759</v>
       </c>
@@ -8445,7 +8471,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>281</v>
       </c>
@@ -8465,7 +8491,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>1091</v>
       </c>
@@ -8484,8 +8510,11 @@
       <c r="F137" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G137" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>1120</v>
       </c>
@@ -8505,7 +8534,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>185</v>
       </c>
@@ -8525,7 +8554,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>150</v>
       </c>
@@ -8545,7 +8574,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>10</v>
       </c>
@@ -8565,7 +8594,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>564</v>
       </c>
@@ -8585,7 +8614,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>71</v>
       </c>
@@ -8604,8 +8633,11 @@
       <c r="F143" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G143" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>1099</v>
       </c>
@@ -8625,7 +8657,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>96</v>
       </c>
@@ -8644,8 +8676,11 @@
       <c r="F145" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G145" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>417</v>
       </c>
@@ -8665,7 +8700,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>1279</v>
       </c>
@@ -8685,7 +8720,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>122</v>
       </c>
@@ -8705,7 +8740,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>895</v>
       </c>
@@ -8725,7 +8760,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>97</v>
       </c>
@@ -8745,7 +8780,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>286</v>
       </c>
@@ -8765,7 +8800,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>640</v>
       </c>
@@ -8785,7 +8820,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>39</v>
       </c>
@@ -8805,7 +8840,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>59</v>
       </c>
@@ -8825,7 +8860,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>317</v>
       </c>
@@ -8845,7 +8880,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>529</v>
       </c>
@@ -8865,7 +8900,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>169</v>
       </c>
@@ -8885,7 +8920,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>152</v>
       </c>
@@ -8905,7 +8940,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>503</v>
       </c>
@@ -8925,7 +8960,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>210</v>
       </c>
@@ -21367,5 +21402,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>